<commit_message>
Uppdaterat med information om vidimering
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/healthcond/actoutcome/trunk/docs/Bilaga MIM_Mappningar_GetReferralOutcome.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/healthcond/actoutcome/trunk/docs/Bilaga MIM_Mappningar_GetReferralOutcome.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="40" windowWidth="27800" windowHeight="15580"/>
+    <workbookView xWindow="600" yWindow="45" windowWidth="27795" windowHeight="15585"/>
   </bookViews>
   <sheets>
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="276">
   <si>
     <t>Meddelandestruktur</t>
   </si>
@@ -815,6 +815,39 @@
   <si>
     <t>Anger typ av svar. Giltiga koder: SR, svar på remissfråga eller SS, slutsvar på remissfråga
 Kodsystem: 1.2.752.97.3.2.8.6</t>
+  </si>
+  <si>
+    <t>attested</t>
+  </si>
+  <si>
+    <t>attestedType</t>
+  </si>
+  <si>
+    <t>TimeStampType</t>
+  </si>
+  <si>
+    <t>Tidpunkten för vidimering</t>
+  </si>
+  <si>
+    <t>attesterHSAId</t>
+  </si>
+  <si>
+    <t>HSA-id för person som vidimerat</t>
+  </si>
+  <si>
+    <t>attesterName</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Namn på person som vidimerat</t>
+  </si>
+  <si>
+    <t>Information om vidimering av enskild utförd åtgärd med tillhörande resultat. Finns attester är åtgärden vidimerad. Med vidimerat menas att information om åtgärden har lästs och den som läst har tagit ansvar.</t>
+  </si>
+  <si>
+    <t>attestedTime</t>
   </si>
 </sst>
 </file>
@@ -880,17 +913,20 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <strike/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -952,7 +988,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1133,6 +1169,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1142,21 +1185,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1464,38 +1510,38 @@
   <sheetPr codeName="Blad2" enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ176"/>
+  <dimension ref="A1:AJ180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X92" sqref="X92:AE92"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB138" sqref="AB138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
-    <col min="2" max="5" width="2.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="2" max="5" width="2.42578125" style="2" customWidth="1"/>
     <col min="6" max="8" width="3" style="2" customWidth="1"/>
-    <col min="9" max="12" width="3.5" style="2" customWidth="1"/>
-    <col min="13" max="17" width="3.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.5" style="2" customWidth="1"/>
+    <col min="9" max="12" width="3.42578125" style="2" customWidth="1"/>
+    <col min="13" max="17" width="3.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" customWidth="1"/>
     <col min="19" max="19" width="9" style="2" customWidth="1"/>
-    <col min="20" max="20" width="21.5" style="2" customWidth="1"/>
-    <col min="21" max="21" width="50.5" style="17" customWidth="1"/>
-    <col min="22" max="22" width="7.5" style="20" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="50.42578125" style="17" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" style="20" customWidth="1"/>
     <col min="23" max="23" width="7" style="20" customWidth="1"/>
-    <col min="24" max="24" width="8.83203125" style="2"/>
-    <col min="25" max="25" width="12.33203125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="11.5" style="2" customWidth="1"/>
-    <col min="27" max="27" width="10.5" style="2" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" style="2"/>
+    <col min="25" max="25" width="12.28515625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" style="2" customWidth="1"/>
     <col min="28" max="28" width="17" style="2" customWidth="1"/>
-    <col min="29" max="29" width="10.5" style="3" customWidth="1"/>
-    <col min="30" max="30" width="12.1640625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="64.33203125" style="19" customWidth="1"/>
-    <col min="32" max="16384" width="8.83203125" style="2"/>
+    <col min="29" max="29" width="10.42578125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="3" customWidth="1"/>
+    <col min="31" max="31" width="64.28515625" style="19" customWidth="1"/>
+    <col min="32" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="2.25" customHeight="1">
+    <row r="1" spans="1:36" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43"/>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -1531,7 +1577,7 @@
       <c r="AG1" s="58"/>
       <c r="AH1" s="20"/>
     </row>
-    <row r="2" spans="1:36" ht="6.75" customHeight="1">
+    <row r="2" spans="1:36" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -1567,49 +1613,49 @@
       <c r="AG2" s="33"/>
       <c r="AH2" s="36"/>
     </row>
-    <row r="3" spans="1:36" ht="27" customHeight="1">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
       <c r="AH3" s="20"/>
       <c r="AI3" s="29"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36" ht="1.5" customHeight="1">
+    <row r="4" spans="1:36" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
@@ -1645,7 +1691,7 @@
       <c r="AG4" s="61"/>
       <c r="AH4" s="36"/>
     </row>
-    <row r="5" spans="1:36" ht="30" customHeight="1">
+    <row r="5" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +1736,7 @@
       <c r="AF5" s="51"/>
       <c r="AG5" s="51"/>
     </row>
-    <row r="6" spans="1:36" ht="1.5" customHeight="1">
+    <row r="6" spans="1:36" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -1725,7 +1771,7 @@
       <c r="AF6" s="40"/>
       <c r="AG6" s="40"/>
     </row>
-    <row r="7" spans="1:36" ht="12.75" customHeight="1">
+    <row r="7" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1798,7 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
     </row>
-    <row r="8" spans="1:36" ht="10.5" customHeight="1">
+    <row r="8" spans="1:36" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>94</v>
       </c>
@@ -1781,7 +1827,7 @@
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1810,7 +1856,7 @@
       </c>
       <c r="W9" s="13"/>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1839,7 +1885,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -1866,7 +1912,7 @@
       <c r="T11" s="4"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -1898,7 +1944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -1934,7 +1980,7 @@
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
     </row>
-    <row r="14" spans="1:36" ht="24">
+    <row r="14" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -1983,7 +2029,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -2021,7 +2067,7 @@
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
     </row>
-    <row r="16" spans="1:36" ht="30.75" customHeight="1">
+    <row r="16" spans="1:36" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -2059,7 +2105,7 @@
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
@@ -2092,7 +2138,7 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
     </row>
-    <row r="18" spans="1:31" ht="36">
+    <row r="18" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -2140,7 +2186,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
@@ -2176,7 +2222,7 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
     </row>
-    <row r="20" spans="1:31" ht="24">
+    <row r="20" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>33</v>
@@ -2224,7 +2270,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="24">
+    <row r="21" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>26</v>
@@ -2260,7 +2306,7 @@
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
@@ -2309,7 +2355,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
         <v>35</v>
@@ -2342,7 +2388,7 @@
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
@@ -2380,7 +2426,7 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
@@ -2417,7 +2463,7 @@
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
         <v>10</v>
@@ -2452,7 +2498,7 @@
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
@@ -2486,7 +2532,7 @@
       <c r="AB27" s="3"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:31" ht="36">
+    <row r="28" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
@@ -2529,7 +2575,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="4"/>
@@ -2563,7 +2609,7 @@
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
     </row>
-    <row r="30" spans="1:31" ht="48">
+    <row r="30" spans="1:31" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
@@ -2602,7 +2648,7 @@
       <c r="AB30" s="3"/>
       <c r="AE30" s="23"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>12</v>
@@ -2646,7 +2692,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
@@ -2682,7 +2728,7 @@
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2731,7 +2777,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -2766,7 +2812,7 @@
       <c r="AB34" s="3"/>
       <c r="AF34" s="22"/>
     </row>
-    <row r="35" spans="1:32" ht="12.75" customHeight="1">
+    <row r="35" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2801,7 +2847,7 @@
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
     </row>
-    <row r="36" spans="1:32" ht="12.75" customHeight="1">
+    <row r="36" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2848,7 +2894,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="12.75" customHeight="1">
+    <row r="37" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2887,7 +2933,7 @@
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
     </row>
-    <row r="38" spans="1:32" ht="24.75" customHeight="1">
+    <row r="38" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2934,7 +2980,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="12.75" customHeight="1">
+    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2968,7 +3014,7 @@
       <c r="AB39" s="3"/>
       <c r="AE39" s="23"/>
     </row>
-    <row r="40" spans="1:32" ht="12.75" customHeight="1">
+    <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3001,7 +3047,7 @@
       <c r="V40" s="11"/>
       <c r="W40" s="11"/>
     </row>
-    <row r="41" spans="1:32" ht="12.75" customHeight="1">
+    <row r="41" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3035,7 +3081,7 @@
       <c r="W41" s="11"/>
       <c r="AE41" s="23"/>
     </row>
-    <row r="42" spans="1:32" ht="12.75" customHeight="1">
+    <row r="42" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3064,7 +3110,7 @@
       <c r="V42" s="11"/>
       <c r="W42" s="11"/>
     </row>
-    <row r="43" spans="1:32" ht="12.75" customHeight="1">
+    <row r="43" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3109,7 +3155,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="12.75" customHeight="1">
+    <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
@@ -3137,7 +3183,7 @@
       <c r="V44" s="11"/>
       <c r="W44" s="11"/>
     </row>
-    <row r="45" spans="1:32" ht="12.75" customHeight="1">
+    <row r="45" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3180,7 +3226,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="12.75" customHeight="1">
+    <row r="46" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3213,7 +3259,7 @@
       <c r="V46" s="18"/>
       <c r="W46" s="18"/>
     </row>
-    <row r="47" spans="1:32" ht="12.75" customHeight="1">
+    <row r="47" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3246,7 +3292,7 @@
       <c r="V47" s="18"/>
       <c r="W47" s="18"/>
     </row>
-    <row r="48" spans="1:32" ht="12.75" customHeight="1">
+    <row r="48" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3292,7 +3338,7 @@
       </c>
       <c r="AF48" s="3"/>
     </row>
-    <row r="49" spans="1:34" ht="12.75" customHeight="1">
+    <row r="49" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3337,7 +3383,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="12.75" customHeight="1">
+    <row r="50" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3383,7 +3429,7 @@
       </c>
       <c r="AF50" s="3"/>
     </row>
-    <row r="51" spans="1:34" ht="12.75" customHeight="1">
+    <row r="51" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3414,7 +3460,7 @@
       <c r="V51" s="11"/>
       <c r="W51" s="11"/>
     </row>
-    <row r="52" spans="1:34" ht="12.75" customHeight="1">
+    <row r="52" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3443,7 +3489,7 @@
       <c r="W52" s="2"/>
       <c r="AE52" s="2"/>
     </row>
-    <row r="53" spans="1:34" ht="12.75" customHeight="1">
+    <row r="53" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -3473,7 +3519,7 @@
       <c r="W53" s="2"/>
       <c r="AE53" s="2"/>
     </row>
-    <row r="54" spans="1:34" ht="12.75" customHeight="1">
+    <row r="54" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -3518,7 +3564,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="12.75" customHeight="1">
+    <row r="55" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -3550,7 +3596,7 @@
       <c r="W55" s="24"/>
       <c r="AE55" s="2"/>
     </row>
-    <row r="56" spans="1:34" ht="24">
+    <row r="56" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>16</v>
@@ -3588,7 +3634,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:34">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
@@ -3619,7 +3665,7 @@
       <c r="AG57" s="27"/>
       <c r="AH57" s="27"/>
     </row>
-    <row r="58" spans="1:34">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3648,7 +3694,7 @@
       <c r="V58" s="11"/>
       <c r="W58" s="11"/>
     </row>
-    <row r="59" spans="1:34">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3691,7 +3737,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:34" ht="24">
+    <row r="60" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3724,7 +3770,7 @@
       <c r="V60" s="26"/>
       <c r="W60" s="26"/>
     </row>
-    <row r="61" spans="1:34">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3759,7 +3805,7 @@
       <c r="W61" s="18"/>
       <c r="AE61" s="2"/>
     </row>
-    <row r="62" spans="1:34">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
         <v>19</v>
@@ -3797,7 +3843,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:34">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="s">
@@ -3825,7 +3871,7 @@
       <c r="V63" s="24"/>
       <c r="W63" s="24"/>
     </row>
-    <row r="64" spans="1:34" ht="24">
+    <row r="64" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3873,7 +3919,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5" t="s">
@@ -3902,7 +3948,7 @@
       <c r="V65" s="11"/>
       <c r="W65" s="11"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3935,7 +3981,7 @@
       <c r="W66" s="11"/>
       <c r="AE66" s="2"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
@@ -3973,7 +4019,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -4018,7 +4064,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -4052,7 +4098,7 @@
       <c r="W69" s="18"/>
       <c r="AE69" s="2"/>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -4084,7 +4130,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:31">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -4112,7 +4158,7 @@
       <c r="V71" s="28"/>
       <c r="W71" s="28"/>
     </row>
-    <row r="72" spans="1:31" ht="24">
+    <row r="72" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -4143,7 +4189,7 @@
       <c r="V72" s="25"/>
       <c r="W72" s="25"/>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -4183,7 +4229,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="74" spans="1:31">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -4216,7 +4262,7 @@
       <c r="V74" s="18"/>
       <c r="W74" s="18"/>
     </row>
-    <row r="75" spans="1:31" ht="24">
+    <row r="75" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="3" t="s">
         <v>54</v>
@@ -4255,7 +4301,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="C76" s="4" t="s">
         <v>55</v>
@@ -4284,7 +4330,7 @@
       <c r="W76" s="18"/>
       <c r="AE76" s="2"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="5" t="s">
@@ -4313,7 +4359,7 @@
       </c>
       <c r="AE77" s="2"/>
     </row>
-    <row r="78" spans="1:31" ht="36">
+    <row r="78" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="C78" s="4"/>
       <c r="E78" s="5" t="s">
@@ -4359,7 +4405,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="C79" s="4"/>
       <c r="E79" s="5" t="s">
@@ -4394,7 +4440,7 @@
       <c r="AA79" s="3"/>
       <c r="AB79" s="3"/>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="C80" s="4"/>
       <c r="E80" s="5" t="s">
@@ -4419,7 +4465,7 @@
       <c r="V80" s="18"/>
       <c r="W80" s="18"/>
     </row>
-    <row r="81" spans="1:34">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="C81" s="4"/>
       <c r="E81" s="5"/>
@@ -4450,7 +4496,7 @@
       <c r="X81" s="3"/>
       <c r="AE81" s="25"/>
     </row>
-    <row r="82" spans="1:34">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -4478,7 +4524,7 @@
       <c r="AB82" s="3"/>
       <c r="AE82" s="23"/>
     </row>
-    <row r="83" spans="1:34">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="C83" s="4"/>
       <c r="E83" s="5"/>
@@ -4500,7 +4546,7 @@
       <c r="V83" s="18"/>
       <c r="W83" s="18"/>
     </row>
-    <row r="84" spans="1:34">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="12" t="s">
         <v>5</v>
@@ -4527,7 +4573,7 @@
       <c r="V84" s="18"/>
       <c r="W84" s="18"/>
     </row>
-    <row r="85" spans="1:34">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="12" t="s">
         <v>21</v>
@@ -4560,7 +4606,7 @@
       <c r="AB85" s="3"/>
       <c r="AE85" s="23"/>
     </row>
-    <row r="86" spans="1:34">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="12" t="s">
         <v>5</v>
@@ -4587,7 +4633,7 @@
       <c r="V86" s="18"/>
       <c r="W86" s="18"/>
     </row>
-    <row r="87" spans="1:34">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
         <v>22</v>
@@ -4616,7 +4662,7 @@
       <c r="V87" s="18"/>
       <c r="W87" s="18"/>
     </row>
-    <row r="88" spans="1:34">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4" t="s">
@@ -4645,7 +4691,7 @@
       <c r="V88" s="11"/>
       <c r="W88" s="11"/>
     </row>
-    <row r="89" spans="1:34">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="12" t="s">
         <v>5</v>
@@ -4670,7 +4716,7 @@
       <c r="V89" s="11"/>
       <c r="W89" s="2"/>
     </row>
-    <row r="90" spans="1:34">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B90" s="12" t="s">
         <v>96</v>
       </c>
@@ -4694,7 +4740,7 @@
       <c r="V90" s="11"/>
       <c r="W90" s="11"/>
     </row>
-    <row r="91" spans="1:34">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B91" s="12" t="s">
         <v>5</v>
       </c>
@@ -4718,7 +4764,7 @@
       <c r="V91" s="11"/>
       <c r="W91" s="11"/>
     </row>
-    <row r="92" spans="1:34">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4" t="s">
@@ -4747,25 +4793,25 @@
       </c>
       <c r="V92" s="11"/>
       <c r="W92" s="11"/>
-      <c r="X92" s="69" t="s">
+      <c r="X92" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="Y92" s="69"/>
-      <c r="Z92" s="69"/>
-      <c r="AA92" s="69"/>
-      <c r="AB92" s="69"/>
-      <c r="AC92" s="70"/>
-      <c r="AD92" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE92" s="71" t="s">
+      <c r="Y92" s="66"/>
+      <c r="Z92" s="66"/>
+      <c r="AA92" s="66"/>
+      <c r="AB92" s="66"/>
+      <c r="AC92" s="67"/>
+      <c r="AD92" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE92" s="68" t="s">
         <v>105</v>
       </c>
       <c r="AF92" s="4"/>
       <c r="AG92" s="4"/>
       <c r="AH92" s="4"/>
     </row>
-    <row r="93" spans="1:34">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -4794,7 +4840,7 @@
       <c r="V93" s="11"/>
       <c r="W93" s="11"/>
     </row>
-    <row r="94" spans="1:34" s="4" customFormat="1">
+    <row r="94" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F94" s="5" t="s">
         <v>9</v>
       </c>
@@ -4818,7 +4864,7 @@
       <c r="AG94" s="2"/>
       <c r="AH94" s="2"/>
     </row>
-    <row r="95" spans="1:34">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -4850,7 +4896,7 @@
       <c r="V95" s="11"/>
       <c r="W95" s="11"/>
     </row>
-    <row r="96" spans="1:34">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -4885,7 +4931,7 @@
       <c r="Y96" s="11"/>
       <c r="AE96" s="2"/>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -4929,7 +4975,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="48">
+    <row r="98" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -4977,7 +5023,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="36">
+    <row r="99" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -5020,7 +5066,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="1:31">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -5049,7 +5095,7 @@
       <c r="V100" s="24"/>
       <c r="W100" s="24"/>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -5085,7 +5131,7 @@
       <c r="AA101" s="3"/>
       <c r="AE101" s="23"/>
     </row>
-    <row r="102" spans="1:31">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -5121,7 +5167,7 @@
       <c r="AA102" s="3"/>
       <c r="AE102" s="23"/>
     </row>
-    <row r="103" spans="1:31">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -5158,7 +5204,7 @@
       <c r="AA103" s="3"/>
       <c r="AE103" s="23"/>
     </row>
-    <row r="104" spans="1:31">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -5194,7 +5240,7 @@
       <c r="AA104" s="3"/>
       <c r="AE104" s="23"/>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -5231,7 +5277,7 @@
       <c r="AA105" s="3"/>
       <c r="AE105" s="23"/>
     </row>
-    <row r="106" spans="1:31">
+    <row r="106" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -5272,7 +5318,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:31">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -5304,7 +5350,7 @@
       <c r="W107" s="24"/>
       <c r="AE107" s="24"/>
     </row>
-    <row r="108" spans="1:31">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -5336,7 +5382,7 @@
       <c r="W108" s="24"/>
       <c r="AE108" s="21"/>
     </row>
-    <row r="109" spans="1:31">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -5379,7 +5425,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -5419,7 +5465,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="111" spans="1:31">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -5449,7 +5495,7 @@
       <c r="W111" s="24"/>
       <c r="AE111" s="35"/>
     </row>
-    <row r="112" spans="1:31">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -5484,7 +5530,7 @@
       <c r="AA112" s="3"/>
       <c r="AE112" s="21"/>
     </row>
-    <row r="113" spans="1:31">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -5517,7 +5563,7 @@
       <c r="Y113" s="3"/>
       <c r="AE113" s="21"/>
     </row>
-    <row r="114" spans="1:31" ht="24">
+    <row r="114" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -5557,7 +5603,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:31">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -5592,7 +5638,7 @@
       <c r="AA115" s="3"/>
       <c r="AE115" s="2"/>
     </row>
-    <row r="116" spans="1:31" ht="24">
+    <row r="116" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -5625,7 +5671,7 @@
       <c r="V116" s="26"/>
       <c r="W116" s="26"/>
     </row>
-    <row r="117" spans="1:31" ht="48">
+    <row r="117" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -5668,7 +5714,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="24">
+    <row r="118" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -5701,7 +5747,7 @@
       <c r="V118" s="11"/>
       <c r="W118" s="11"/>
     </row>
-    <row r="119" spans="1:31">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -5732,7 +5778,7 @@
       <c r="V119" s="11"/>
       <c r="W119" s="11"/>
     </row>
-    <row r="120" spans="1:31">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -5763,7 +5809,7 @@
       <c r="V120" s="11"/>
       <c r="W120" s="11"/>
     </row>
-    <row r="121" spans="1:31" ht="24">
+    <row r="121" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -5796,7 +5842,7 @@
       <c r="V121" s="24"/>
       <c r="W121" s="24"/>
     </row>
-    <row r="122" spans="1:31" ht="36">
+    <row r="122" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -5838,7 +5884,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:31" ht="24">
+    <row r="123" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5879,7 +5925,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="1:31">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5908,7 +5954,7 @@
       <c r="W124" s="11"/>
       <c r="Y124" s="3"/>
     </row>
-    <row r="125" spans="1:31">
+    <row r="125" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -5947,7 +5993,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:31">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -5977,7 +6023,7 @@
       <c r="V126" s="11"/>
       <c r="W126" s="11"/>
     </row>
-    <row r="127" spans="1:31">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -6003,7 +6049,7 @@
       <c r="T127" s="6"/>
       <c r="U127" s="8"/>
     </row>
-    <row r="128" spans="1:31">
+    <row r="128" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -6031,7 +6077,7 @@
       <c r="V128" s="24"/>
       <c r="W128" s="24"/>
     </row>
-    <row r="129" spans="1:31">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -6059,7 +6105,7 @@
       <c r="V129" s="24"/>
       <c r="W129" s="24"/>
     </row>
-    <row r="130" spans="1:31">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -6086,7 +6132,7 @@
       <c r="V130" s="11"/>
       <c r="W130" s="11"/>
     </row>
-    <row r="131" spans="1:31">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -6119,7 +6165,7 @@
       <c r="Z131" s="32"/>
       <c r="AE131" s="8"/>
     </row>
-    <row r="132" spans="1:31">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -6148,7 +6194,7 @@
       <c r="V132" s="18"/>
       <c r="W132" s="18"/>
     </row>
-    <row r="133" spans="1:31" ht="24">
+    <row r="133" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6190,7 +6236,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="134" spans="1:31">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -6218,7 +6264,7 @@
       <c r="V134" s="11"/>
       <c r="W134" s="11"/>
     </row>
-    <row r="135" spans="1:31">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -6246,7 +6292,7 @@
       <c r="V135" s="11"/>
       <c r="W135" s="11"/>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -6254,28 +6300,38 @@
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
       <c r="G136" s="4"/>
-      <c r="H136" s="6"/>
+      <c r="H136" s="4"/>
       <c r="I136" s="4"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="5"/>
-      <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
+      <c r="J136" s="5"/>
       <c r="N136" s="4"/>
       <c r="O136" s="4"/>
       <c r="P136" s="4"/>
       <c r="Q136" s="4"/>
       <c r="R136" s="4"/>
       <c r="S136" s="5"/>
-      <c r="T136" s="6"/>
+      <c r="T136" s="5"/>
       <c r="U136" s="8"/>
       <c r="V136" s="11"/>
       <c r="W136" s="11"/>
-    </row>
-    <row r="137" spans="1:31">
+      <c r="Y136" s="72" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z136" s="72"/>
+      <c r="AA136" s="72"/>
+      <c r="AB136" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="AC136" s="72"/>
+      <c r="AD136" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE136" s="72" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="137" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A137" s="4"/>
-      <c r="B137" s="12" t="s">
-        <v>210</v>
-      </c>
+      <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -6283,26 +6339,36 @@
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="4"/>
-      <c r="M137" s="4"/>
+      <c r="J137" s="5"/>
       <c r="N137" s="4"/>
       <c r="O137" s="4"/>
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
       <c r="R137" s="4"/>
-      <c r="S137" s="4"/>
-      <c r="T137" s="4"/>
-      <c r="U137" s="15"/>
+      <c r="S137" s="5"/>
+      <c r="T137" s="5"/>
+      <c r="U137" s="8"/>
       <c r="V137" s="11"/>
       <c r="W137" s="11"/>
-    </row>
-    <row r="138" spans="1:31">
+      <c r="Y137" s="74"/>
+      <c r="Z137" s="72" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA137" s="72"/>
+      <c r="AB137" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="AC137" s="74"/>
+      <c r="AD137" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE137" s="75" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="138" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A138" s="4"/>
-      <c r="B138" s="12" t="s">
-        <v>133</v>
-      </c>
+      <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -6310,24 +6376,36 @@
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
-      <c r="M138" s="4"/>
+      <c r="J138" s="5"/>
       <c r="N138" s="4"/>
       <c r="O138" s="4"/>
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
       <c r="R138" s="4"/>
-      <c r="S138" s="4"/>
-      <c r="T138" s="4"/>
-      <c r="U138" s="15"/>
-    </row>
-    <row r="139" spans="1:31">
+      <c r="S138" s="5"/>
+      <c r="T138" s="5"/>
+      <c r="U138" s="8"/>
+      <c r="V138" s="11"/>
+      <c r="W138" s="11"/>
+      <c r="Y138" s="74"/>
+      <c r="Z138" s="72" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA138" s="72"/>
+      <c r="AB138" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC138" s="74"/>
+      <c r="AD138" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE138" s="75" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="139" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A139" s="4"/>
-      <c r="B139" s="12" t="s">
-        <v>210</v>
-      </c>
+      <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -6335,35 +6413,45 @@
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
+      <c r="J139" s="5"/>
       <c r="N139" s="4"/>
       <c r="O139" s="4"/>
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
       <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
-      <c r="U139" s="15"/>
+      <c r="S139" s="5"/>
+      <c r="T139" s="5"/>
+      <c r="U139" s="8"/>
       <c r="V139" s="11"/>
       <c r="W139" s="11"/>
-    </row>
-    <row r="140" spans="1:31">
+      <c r="Y139" s="74"/>
+      <c r="Z139" s="72" t="s">
+        <v>271</v>
+      </c>
+      <c r="AA139" s="72"/>
+      <c r="AB139" s="74"/>
+      <c r="AC139" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD139" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE139" s="75" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
-      <c r="D140" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="D140" s="4"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
+      <c r="H140" s="6"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
+      <c r="K140" s="5"/>
       <c r="L140" s="4"/>
       <c r="M140" s="4"/>
       <c r="N140" s="4"/>
@@ -6371,180 +6459,143 @@
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
-      <c r="S140" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T140" s="4"/>
+      <c r="S140" s="5"/>
+      <c r="T140" s="6"/>
       <c r="U140" s="8"/>
       <c r="V140" s="11"/>
-      <c r="W140" s="18"/>
-      <c r="X140" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y140" s="3"/>
-      <c r="Z140" s="3"/>
-      <c r="AA140" s="3"/>
-      <c r="AB140" s="3"/>
-      <c r="AD140" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE140" s="19" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="141" spans="1:31">
+      <c r="W140" s="11"/>
+    </row>
+    <row r="141" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
+      <c r="B141" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
-      <c r="E141" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E141" s="4"/>
       <c r="F141" s="4"/>
-      <c r="G141" s="5"/>
+      <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
       <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="4"/>
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
-      <c r="S141" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="S141" s="4"/>
       <c r="T141" s="4"/>
-      <c r="U141" s="7"/>
+      <c r="U141" s="15"/>
       <c r="V141" s="11"/>
-      <c r="W141" s="18"/>
-      <c r="X141" s="3"/>
-      <c r="Y141" s="3"/>
-      <c r="Z141" s="3"/>
-      <c r="AA141" s="3"/>
-      <c r="AB141" s="3"/>
-    </row>
-    <row r="142" spans="1:31" ht="24">
+      <c r="W141" s="11"/>
+    </row>
+    <row r="142" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
+      <c r="B142" s="12" t="s">
+        <v>133</v>
+      </c>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
-      <c r="F142" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="F142" s="4"/>
       <c r="G142" s="4"/>
-      <c r="H142" s="5"/>
+      <c r="H142" s="4"/>
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
       <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
-      <c r="S142" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="S142" s="4"/>
       <c r="T142" s="4"/>
-      <c r="U142" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="V142" s="11"/>
-      <c r="W142" s="18"/>
-      <c r="X142" s="3"/>
-      <c r="Y142" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z142" s="3"/>
-      <c r="AA142" s="3"/>
-      <c r="AB142" s="3"/>
-      <c r="AC142" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD142" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE142" s="19" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="143" spans="1:31">
+      <c r="U142" s="15"/>
+    </row>
+    <row r="143" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
+      <c r="B143" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
-      <c r="G143" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H143" s="5"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
-      <c r="S143" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T143" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="U143" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="V143" s="18"/>
-      <c r="W143" s="18"/>
-      <c r="X143" s="3"/>
-      <c r="Y143" s="3"/>
-      <c r="Z143" s="3"/>
-      <c r="AA143" s="3"/>
-      <c r="AB143" s="3"/>
-    </row>
-    <row r="144" spans="1:31" ht="24">
+      <c r="S143" s="4"/>
+      <c r="T143" s="4"/>
+      <c r="U143" s="15"/>
+      <c r="V143" s="11"/>
+      <c r="W143" s="11"/>
+    </row>
+    <row r="144" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
-      <c r="G144" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
       <c r="J144" s="4"/>
       <c r="K144" s="4"/>
       <c r="L144" s="4"/>
       <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
       <c r="S144" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="T144" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="U144" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="V144" s="24"/>
-      <c r="W144" s="24"/>
-      <c r="X144" s="3"/>
+      <c r="T144" s="4"/>
+      <c r="U144" s="8"/>
+      <c r="V144" s="11"/>
+      <c r="W144" s="18"/>
+      <c r="X144" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="Y144" s="3"/>
       <c r="Z144" s="3"/>
       <c r="AA144" s="3"/>
       <c r="AB144" s="3"/>
-    </row>
-    <row r="145" spans="1:31">
+      <c r="AD144" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE144" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="145" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A145" s="4"/>
-      <c r="E145" s="4"/>
-      <c r="F145" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F145" s="4"/>
+      <c r="G145" s="5"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
@@ -6557,23 +6608,27 @@
       <c r="S145" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="U145" s="15"/>
-      <c r="V145" s="24"/>
-      <c r="W145" s="24"/>
+      <c r="T145" s="4"/>
+      <c r="U145" s="7"/>
+      <c r="V145" s="11"/>
+      <c r="W145" s="18"/>
       <c r="X145" s="3"/>
       <c r="Y145" s="3"/>
       <c r="Z145" s="3"/>
       <c r="AA145" s="3"/>
       <c r="AB145" s="3"/>
     </row>
-    <row r="146" spans="1:31">
+    <row r="146" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
       <c r="E146" s="4"/>
-      <c r="F146" s="4"/>
-      <c r="G146" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H146" s="4"/>
+      <c r="F146" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G146" s="4"/>
+      <c r="H146" s="5"/>
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
@@ -6582,31 +6637,41 @@
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
       <c r="R146" s="4"/>
-      <c r="S146" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T146" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="U146" s="14" t="s">
-        <v>144</v>
+      <c r="S146" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T146" s="4"/>
+      <c r="U146" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="V146" s="11"/>
       <c r="W146" s="18"/>
       <c r="X146" s="3"/>
-      <c r="Y146" s="3"/>
+      <c r="Y146" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="Z146" s="3"/>
       <c r="AA146" s="3"/>
       <c r="AB146" s="3"/>
-    </row>
-    <row r="147" spans="1:31">
+      <c r="AC146" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD146" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE146" s="19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="147" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
-      <c r="G147" s="3" t="s">
-        <v>31</v>
+      <c r="F147" s="4"/>
+      <c r="G147" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="H147" s="5"/>
       <c r="I147" s="4"/>
@@ -6620,10 +6685,12 @@
       <c r="S147" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="T147" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="U147" s="8"/>
+      <c r="T147" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="U147" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="V147" s="18"/>
       <c r="W147" s="18"/>
       <c r="X147" s="3"/>
@@ -6632,17 +6699,15 @@
       <c r="AA147" s="3"/>
       <c r="AB147" s="3"/>
     </row>
-    <row r="148" spans="1:31" ht="36">
+    <row r="148" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A148" s="4"/>
-      <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
       <c r="E148" s="4"/>
-      <c r="F148" s="5" t="s">
-        <v>46</v>
+      <c r="F148" s="4"/>
+      <c r="G148" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="H148" s="4"/>
-      <c r="I148" s="5"/>
+      <c r="I148" s="4"/>
       <c r="J148" s="4"/>
       <c r="K148" s="4"/>
       <c r="L148" s="4"/>
@@ -6650,45 +6715,32 @@
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
       <c r="R148" s="4"/>
-      <c r="S148" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T148" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U148" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="V148" s="18"/>
-      <c r="W148" s="18"/>
+      <c r="S148" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T148" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U148" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="V148" s="24"/>
+      <c r="W148" s="24"/>
       <c r="X148" s="3"/>
-      <c r="Y148" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="Y148" s="3"/>
       <c r="Z148" s="3"/>
       <c r="AA148" s="3"/>
       <c r="AB148" s="3"/>
-      <c r="AC148" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD148" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE148" s="28" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="149" spans="1:31">
+    </row>
+    <row r="149" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
       <c r="E149" s="4"/>
-      <c r="F149" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F149" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G149" s="4"/>
       <c r="H149" s="4"/>
-      <c r="I149" s="5"/>
+      <c r="I149" s="4"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
@@ -6696,12 +6748,10 @@
       <c r="P149" s="4"/>
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
-      <c r="S149" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U149" s="7" t="s">
-        <v>122</v>
-      </c>
+      <c r="S149" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U149" s="15"/>
       <c r="V149" s="24"/>
       <c r="W149" s="24"/>
       <c r="X149" s="3"/>
@@ -6710,17 +6760,15 @@
       <c r="AA149" s="3"/>
       <c r="AB149" s="3"/>
     </row>
-    <row r="150" spans="1:31">
+    <row r="150" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
       <c r="E150" s="4"/>
-      <c r="G150" s="3" t="s">
-        <v>123</v>
+      <c r="F150" s="4"/>
+      <c r="G150" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="H150" s="4"/>
-      <c r="I150" s="5"/>
+      <c r="I150" s="4"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
@@ -6731,28 +6779,31 @@
       <c r="S150" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T150" s="3"/>
-      <c r="U150" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="W150" s="26"/>
+      <c r="T150" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U150" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="V150" s="11"/>
+      <c r="W150" s="18"/>
       <c r="X150" s="3"/>
       <c r="Y150" s="3"/>
       <c r="Z150" s="3"/>
       <c r="AA150" s="3"/>
       <c r="AB150" s="3"/>
     </row>
-    <row r="151" spans="1:31">
+    <row r="151" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
-      <c r="G151" s="3"/>
-      <c r="H151" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I151" s="5"/>
+      <c r="G151" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H151" s="5"/>
+      <c r="I151" s="4"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
@@ -6761,44 +6812,31 @@
       <c r="Q151" s="4"/>
       <c r="R151" s="4"/>
       <c r="S151" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T151" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U151" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="W151" s="26"/>
+        <v>1</v>
+      </c>
+      <c r="T151" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="U151" s="8"/>
+      <c r="V151" s="18"/>
+      <c r="W151" s="18"/>
       <c r="X151" s="3"/>
-      <c r="Y151" s="3" t="s">
-        <v>212</v>
-      </c>
+      <c r="Y151" s="3"/>
       <c r="Z151" s="3"/>
       <c r="AA151" s="3"/>
       <c r="AB151" s="3"/>
-      <c r="AC151" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD151" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE151" s="19" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="152" spans="1:31">
+    </row>
+    <row r="152" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H152" s="5"/>
-      <c r="I152" s="4"/>
+      <c r="F152" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H152" s="4"/>
+      <c r="I152" s="5"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
@@ -6809,88 +6847,87 @@
       <c r="S152" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T152" s="4"/>
-      <c r="U152" s="8"/>
-      <c r="W152" s="26"/>
+      <c r="T152" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U152" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="V152" s="18"/>
+      <c r="W152" s="18"/>
       <c r="X152" s="3"/>
-      <c r="Y152" s="3"/>
+      <c r="Y152" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="Z152" s="3"/>
       <c r="AA152" s="3"/>
       <c r="AB152" s="3"/>
-    </row>
-    <row r="153" spans="1:31">
+      <c r="AC152" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD152" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE152" s="28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="153" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="4"/>
-      <c r="G153" s="4"/>
-      <c r="H153" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I153" s="4"/>
+      <c r="F153" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H153" s="4"/>
+      <c r="I153" s="5"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
       <c r="L153" s="4"/>
       <c r="M153" s="4"/>
-      <c r="N153" s="4"/>
-      <c r="O153" s="4"/>
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
       <c r="R153" s="4"/>
       <c r="S153" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T153" s="4"/>
-      <c r="U153" s="15"/>
-      <c r="W153" s="26"/>
+      <c r="U153" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="V153" s="24"/>
+      <c r="W153" s="24"/>
       <c r="X153" s="3"/>
-      <c r="Y153" s="3" t="s">
-        <v>232</v>
-      </c>
+      <c r="Y153" s="3"/>
       <c r="Z153" s="3"/>
       <c r="AA153" s="3"/>
       <c r="AB153" s="3"/>
-      <c r="AC153" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD153" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE153" s="19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="154" spans="1:31">
+    </row>
+    <row r="154" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
-      <c r="F154" s="4"/>
-      <c r="G154" s="4"/>
+      <c r="G154" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="H154" s="4"/>
-      <c r="I154" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="I154" s="5"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
       <c r="M154" s="4"/>
-      <c r="N154" s="4"/>
-      <c r="O154" s="4"/>
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
       <c r="R154" s="4"/>
       <c r="S154" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T154" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="U154" s="15" t="s">
-        <v>124</v>
+      <c r="T154" s="3"/>
+      <c r="U154" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="W154" s="26"/>
       <c r="X154" s="3"/>
@@ -6898,69 +6935,76 @@
       <c r="Z154" s="3"/>
       <c r="AA154" s="3"/>
       <c r="AB154" s="3"/>
-      <c r="AE154" s="2"/>
-    </row>
-    <row r="155" spans="1:31">
+    </row>
+    <row r="155" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
-      <c r="F155" s="4"/>
-      <c r="G155" s="4"/>
-      <c r="H155" s="4"/>
-      <c r="I155" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="G155" s="3"/>
+      <c r="H155" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I155" s="5"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
       <c r="L155" s="4"/>
       <c r="M155" s="4"/>
-      <c r="N155" s="4"/>
-      <c r="O155" s="4"/>
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
       <c r="S155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T155" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U155" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="T155" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U155" s="31" t="s">
+        <v>145</v>
+      </c>
       <c r="W155" s="26"/>
       <c r="X155" s="3"/>
-      <c r="Y155" s="3"/>
+      <c r="Y155" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="Z155" s="3"/>
       <c r="AA155" s="3"/>
       <c r="AB155" s="3"/>
-    </row>
-    <row r="156" spans="1:31">
+      <c r="AC155" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD155" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE155" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="156" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
       <c r="F156" s="4"/>
-      <c r="G156" s="4"/>
-      <c r="H156" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="G156" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H156" s="5"/>
       <c r="I156" s="4"/>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
       <c r="L156" s="4"/>
       <c r="M156" s="4"/>
-      <c r="N156" s="4"/>
-      <c r="O156" s="4"/>
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
       <c r="R156" s="4"/>
-      <c r="S156" s="5" t="s">
+      <c r="S156" s="6" t="s">
         <v>1</v>
       </c>
       <c r="T156" s="4"/>
-      <c r="U156" s="15"/>
+      <c r="U156" s="8"/>
       <c r="W156" s="26"/>
       <c r="X156" s="3"/>
       <c r="Y156" s="3"/>
@@ -6968,18 +7012,18 @@
       <c r="AA156" s="3"/>
       <c r="AB156" s="3"/>
     </row>
-    <row r="157" spans="1:31">
+    <row r="157" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
       <c r="F157" s="4"/>
-      <c r="G157" s="5"/>
-      <c r="H157" s="4"/>
-      <c r="I157" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="G157" s="4"/>
+      <c r="H157" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I157" s="4"/>
       <c r="J157" s="4"/>
       <c r="K157" s="4"/>
       <c r="L157" s="4"/>
@@ -6988,34 +7032,31 @@
       <c r="O157" s="4"/>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
-      <c r="S157" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T157" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="U157" s="14" t="s">
-        <v>103</v>
-      </c>
+      <c r="R157" s="4"/>
+      <c r="S157" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T157" s="4"/>
+      <c r="U157" s="15"/>
       <c r="W157" s="26"/>
       <c r="X157" s="3"/>
       <c r="Y157" s="3" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="Z157" s="3"/>
       <c r="AA157" s="3"/>
       <c r="AB157" s="3"/>
       <c r="AC157" s="3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="AD157" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE157" s="19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="158" spans="1:31">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="158" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -7023,10 +7064,10 @@
       <c r="E158" s="4"/>
       <c r="F158" s="4"/>
       <c r="G158" s="4"/>
-      <c r="H158" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I158" s="4"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
@@ -7035,19 +7076,25 @@
       <c r="O158" s="4"/>
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
-      <c r="S158" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T158" s="4"/>
-      <c r="U158" s="15"/>
+      <c r="R158" s="4"/>
+      <c r="S158" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T158" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U158" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="W158" s="26"/>
       <c r="X158" s="3"/>
       <c r="Y158" s="3"/>
       <c r="Z158" s="3"/>
       <c r="AA158" s="3"/>
       <c r="AB158" s="3"/>
-    </row>
-    <row r="159" spans="1:31" ht="24">
+      <c r="AE158" s="2"/>
+    </row>
+    <row r="159" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -7055,9 +7102,9 @@
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
       <c r="G159" s="4"/>
-      <c r="H159" s="5"/>
-      <c r="I159" s="6" t="s">
-        <v>3</v>
+      <c r="H159" s="4"/>
+      <c r="I159" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
@@ -7067,32 +7114,22 @@
       <c r="O159" s="4"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
-      <c r="S159" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T159" s="4"/>
-      <c r="U159" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="R159" s="4"/>
+      <c r="S159" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T159" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U159" s="15"/>
       <c r="W159" s="26"/>
       <c r="X159" s="3"/>
-      <c r="Y159" s="3" t="s">
-        <v>247</v>
-      </c>
+      <c r="Y159" s="3"/>
       <c r="Z159" s="3"/>
       <c r="AA159" s="3"/>
       <c r="AB159" s="3"/>
-      <c r="AC159" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD159" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE159" s="23" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="160" spans="1:31" ht="24">
+    </row>
+    <row r="160" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
@@ -7100,11 +7137,11 @@
       <c r="E160" s="4"/>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
-      <c r="H160" s="5"/>
+      <c r="H160" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I160" s="4"/>
-      <c r="J160" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="J160" s="4"/>
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
       <c r="M160" s="4"/>
@@ -7112,36 +7149,33 @@
       <c r="O160" s="4"/>
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
-      <c r="S160" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T160" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="U160" s="15" t="s">
-        <v>126</v>
-      </c>
+      <c r="R160" s="4"/>
+      <c r="S160" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T160" s="4"/>
+      <c r="U160" s="15"/>
       <c r="W160" s="26"/>
       <c r="X160" s="3"/>
       <c r="Y160" s="3"/>
       <c r="Z160" s="3"/>
       <c r="AA160" s="3"/>
       <c r="AB160" s="3"/>
-      <c r="AE160" s="2"/>
-    </row>
-    <row r="161" spans="1:31">
+    </row>
+    <row r="161" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
       <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
+      <c r="G161" s="5"/>
       <c r="H161" s="4"/>
-      <c r="I161" s="5"/>
-      <c r="J161" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="I161" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
       <c r="L161" s="4"/>
       <c r="M161" s="4"/>
       <c r="N161" s="4"/>
@@ -7149,22 +7183,33 @@
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
       <c r="S161" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T161" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U161" s="7" t="s">
-        <v>149</v>
+        <v>2</v>
+      </c>
+      <c r="T161" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U161" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="W161" s="26"/>
       <c r="X161" s="3"/>
-      <c r="Y161" s="3"/>
+      <c r="Y161" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="Z161" s="3"/>
       <c r="AA161" s="3"/>
       <c r="AB161" s="3"/>
-    </row>
-    <row r="162" spans="1:31">
+      <c r="AC161" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD161" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE161" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="162" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
@@ -7172,10 +7217,10 @@
       <c r="E162" s="4"/>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="H162" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I162" s="4"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
@@ -7185,33 +7230,18 @@
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
       <c r="S162" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T162" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="U162" s="7" t="s">
-        <v>127</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T162" s="4"/>
+      <c r="U162" s="15"/>
       <c r="W162" s="26"/>
       <c r="X162" s="3"/>
-      <c r="Y162" s="3" t="s">
-        <v>248</v>
-      </c>
+      <c r="Y162" s="3"/>
       <c r="Z162" s="3"/>
       <c r="AA162" s="3"/>
       <c r="AB162" s="3"/>
-      <c r="AC162" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD162" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE162" s="19" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="163" spans="1:31" ht="24">
+    </row>
+    <row r="163" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -7220,8 +7250,8 @@
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="5"/>
-      <c r="I163" s="4" t="s">
-        <v>51</v>
+      <c r="I163" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
@@ -7232,33 +7262,31 @@
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
       <c r="S163" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T163" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="U163" s="7" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="T163" s="4"/>
+      <c r="U163" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="W163" s="26"/>
       <c r="X163" s="3"/>
       <c r="Y163" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Z163" s="3"/>
       <c r="AA163" s="3"/>
       <c r="AB163" s="3"/>
       <c r="AC163" s="3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="AD163" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE163" s="19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="164" spans="1:31">
+        <v>111</v>
+      </c>
+      <c r="AE163" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="164" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -7266,11 +7294,11 @@
       <c r="E164" s="4"/>
       <c r="F164" s="4"/>
       <c r="G164" s="4"/>
-      <c r="H164" s="4"/>
-      <c r="I164" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J164" s="4"/>
+      <c r="H164" s="5"/>
+      <c r="I164" s="4"/>
+      <c r="J164" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
       <c r="M164" s="4"/>
@@ -7279,46 +7307,35 @@
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
       <c r="S164" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T164" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T164" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="U164" s="7" t="s">
-        <v>81</v>
+      <c r="U164" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="W164" s="26"/>
       <c r="X164" s="3"/>
-      <c r="Y164" s="3" t="s">
-        <v>250</v>
-      </c>
+      <c r="Y164" s="3"/>
       <c r="Z164" s="3"/>
       <c r="AA164" s="3"/>
       <c r="AB164" s="3"/>
-      <c r="AC164" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD164" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE164" s="19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="165" spans="1:31">
+      <c r="AE164" s="2"/>
+    </row>
+    <row r="165" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
-      <c r="F165" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="F165" s="4"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
       <c r="I165" s="5"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
+      <c r="J165" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="L165" s="4"/>
       <c r="M165" s="4"/>
       <c r="N165" s="4"/>
@@ -7326,37 +7343,33 @@
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
       <c r="S165" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="T165" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="U165" s="7" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="W165" s="26"/>
       <c r="X165" s="3"/>
-      <c r="Y165" s="3" t="s">
-        <v>251</v>
-      </c>
+      <c r="Y165" s="3"/>
       <c r="Z165" s="3"/>
       <c r="AA165" s="3"/>
       <c r="AB165" s="3"/>
-      <c r="AD165" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE165" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="166" spans="1:31">
+    </row>
+    <row r="166" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
-      <c r="G166" s="3" t="s">
-        <v>128</v>
-      </c>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
       <c r="H166" s="4"/>
-      <c r="I166" s="5"/>
+      <c r="I166" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
@@ -7366,17 +7379,33 @@
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
       <c r="S166" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="U166" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="T166" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="U166" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="W166" s="26"/>
       <c r="X166" s="3"/>
-      <c r="Y166" s="3"/>
+      <c r="Y166" s="3" t="s">
+        <v>248</v>
+      </c>
       <c r="Z166" s="3"/>
       <c r="AA166" s="3"/>
       <c r="AB166" s="3"/>
-    </row>
-    <row r="167" spans="1:31">
+      <c r="AC166" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD166" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE166" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="167" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -7384,10 +7413,10 @@
       <c r="E167" s="4"/>
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
-      <c r="H167" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I167" s="5"/>
+      <c r="H167" s="5"/>
+      <c r="I167" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
@@ -7397,20 +7426,33 @@
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
       <c r="S167" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T167" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="U167" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="T167" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U167" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="W167" s="26"/>
       <c r="X167" s="3"/>
-      <c r="Y167" s="3"/>
+      <c r="Y167" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="Z167" s="3"/>
       <c r="AA167" s="3"/>
       <c r="AB167" s="3"/>
-    </row>
-    <row r="168" spans="1:31">
+      <c r="AC167" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD167" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE167" s="19" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="168" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -7418,10 +7460,10 @@
       <c r="E168" s="4"/>
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
-      <c r="H168" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I168" s="4"/>
+      <c r="H168" s="4"/>
+      <c r="I168" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
@@ -7431,31 +7473,45 @@
       <c r="P168" s="4"/>
       <c r="Q168" s="4"/>
       <c r="S168" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T168" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U168" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="T168" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U168" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="W168" s="26"/>
       <c r="X168" s="3"/>
-      <c r="Y168" s="3"/>
+      <c r="Y168" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="Z168" s="3"/>
       <c r="AA168" s="3"/>
       <c r="AB168" s="3"/>
-    </row>
-    <row r="169" spans="1:31" ht="36">
+      <c r="AC168" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD168" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE168" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="169" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
-      <c r="F169" s="4"/>
+      <c r="F169" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G169" s="4"/>
-      <c r="H169" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I169" s="4"/>
+      <c r="H169" s="4"/>
+      <c r="I169" s="5"/>
+      <c r="J169" s="4"/>
       <c r="K169" s="4"/>
       <c r="L169" s="4"/>
       <c r="M169" s="4"/>
@@ -7463,43 +7519,50 @@
       <c r="O169" s="4"/>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
-      <c r="S169" s="3"/>
-      <c r="T169" s="4"/>
-      <c r="U169" s="8" t="s">
-        <v>132</v>
+      <c r="S169" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U169" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="W169" s="26"/>
       <c r="X169" s="3"/>
-      <c r="Y169" s="3"/>
-      <c r="Z169" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="Y169" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z169" s="3"/>
       <c r="AA169" s="3"/>
       <c r="AB169" s="3"/>
-      <c r="AC169" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="AD169" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE169" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="170" spans="1:31">
+        <v>2</v>
+      </c>
+      <c r="AE169" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="170" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A170" s="4"/>
-      <c r="I170" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4"/>
+      <c r="G170" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="5"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="4"/>
+      <c r="L170" s="4"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
       <c r="S170" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T170" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U170" s="14" t="s">
-        <v>131</v>
-      </c>
+      <c r="U170" s="7"/>
       <c r="W170" s="26"/>
       <c r="X170" s="3"/>
       <c r="Y170" s="3"/>
@@ -7507,20 +7570,33 @@
       <c r="AA170" s="3"/>
       <c r="AB170" s="3"/>
     </row>
-    <row r="171" spans="1:31" ht="24">
+    <row r="171" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A171" s="4"/>
-      <c r="I171" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I171" s="5"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
       <c r="S171" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T171" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="U171" s="34" t="s">
-        <v>221</v>
-      </c>
+      <c r="T171" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="U171" s="7"/>
       <c r="W171" s="26"/>
       <c r="X171" s="3"/>
       <c r="Y171" s="3"/>
@@ -7528,58 +7604,96 @@
       <c r="AA171" s="3"/>
       <c r="AB171" s="3"/>
     </row>
-    <row r="172" spans="1:31" ht="24">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A172" s="4"/>
-      <c r="H172" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I172" s="4"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
       <c r="S172" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U172" s="14" t="s">
-        <v>151</v>
-      </c>
+      <c r="T172" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U172" s="8"/>
       <c r="W172" s="26"/>
       <c r="X172" s="3"/>
       <c r="Y172" s="3"/>
-      <c r="Z172" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="Z172" s="3"/>
       <c r="AA172" s="3"/>
       <c r="AB172" s="3"/>
-      <c r="AC172" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD172" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE172" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="173" spans="1:31" ht="26.25" customHeight="1">
+    </row>
+    <row r="173" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A173" s="4"/>
-      <c r="I173" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S173" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T173" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U173" s="14" t="s">
-        <v>89</v>
+      <c r="B173" s="4"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
+      <c r="H173" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I173" s="4"/>
+      <c r="K173" s="4"/>
+      <c r="L173" s="4"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="4"/>
+      <c r="O173" s="4"/>
+      <c r="P173" s="4"/>
+      <c r="Q173" s="4"/>
+      <c r="S173" s="3"/>
+      <c r="T173" s="4"/>
+      <c r="U173" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="W173" s="26"/>
       <c r="X173" s="3"/>
       <c r="Y173" s="3"/>
-      <c r="Z173" s="3"/>
+      <c r="Z173" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="AA173" s="3"/>
       <c r="AB173" s="3"/>
-    </row>
-    <row r="174" spans="1:31">
+      <c r="AC173" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD173" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE173" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="174" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A174" s="4"/>
+      <c r="I174" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T174" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U174" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="W174" s="26"/>
       <c r="X174" s="3"/>
       <c r="Y174" s="3"/>
@@ -7587,8 +7701,20 @@
       <c r="AA174" s="3"/>
       <c r="AB174" s="3"/>
     </row>
-    <row r="175" spans="1:31">
+    <row r="175" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A175" s="4"/>
+      <c r="I175" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S175" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T175" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U175" s="34" t="s">
+        <v>221</v>
+      </c>
       <c r="W175" s="26"/>
       <c r="X175" s="3"/>
       <c r="Y175" s="3"/>
@@ -7596,13 +7722,81 @@
       <c r="AA175" s="3"/>
       <c r="AB175" s="3"/>
     </row>
-    <row r="176" spans="1:31">
+    <row r="176" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A176" s="4"/>
+      <c r="H176" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S176" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U176" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="W176" s="26"/>
       <c r="X176" s="3"/>
       <c r="Y176" s="3"/>
-      <c r="Z176" s="3"/>
+      <c r="Z176" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="AA176" s="3"/>
       <c r="AB176" s="3"/>
+      <c r="AC176" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD176" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE176" s="21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="177" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="I177" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S177" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T177" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U177" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="W177" s="26"/>
+      <c r="X177" s="3"/>
+      <c r="Y177" s="3"/>
+      <c r="Z177" s="3"/>
+      <c r="AA177" s="3"/>
+      <c r="AB177" s="3"/>
+    </row>
+    <row r="178" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="W178" s="26"/>
+      <c r="X178" s="3"/>
+      <c r="Y178" s="3"/>
+      <c r="Z178" s="3"/>
+      <c r="AA178" s="3"/>
+      <c r="AB178" s="3"/>
+    </row>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="W179" s="26"/>
+      <c r="X179" s="3"/>
+      <c r="Y179" s="3"/>
+      <c r="Z179" s="3"/>
+      <c r="AA179" s="3"/>
+      <c r="AB179" s="3"/>
+    </row>
+    <row r="180" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W180" s="26"/>
+      <c r="X180" s="3"/>
+      <c r="Y180" s="3"/>
+      <c r="Z180" s="3"/>
+      <c r="AA180" s="3"/>
+      <c r="AB180" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>